<commit_message>
# 101 sms service # 100 statistic for days off # 66 excel export
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/Projects.xlsx
+++ b/src/main/resources/excel/Projects.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>Project Name</t>
   </si>
@@ -38,34 +38,115 @@
     <t>Created</t>
   </si>
   <si>
-    <t># 12 LRMP</t>
+    <t># 54 LRPM</t>
   </si>
   <si>
     <t>Kyiv</t>
   </si>
   <si>
-    <t>2017-04-25</t>
-  </si>
-  <si>
-    <t>2017-06-11</t>
-  </si>
-  <si>
-    <t>Igor Hnes</t>
-  </si>
-  <si>
-    <t>Lada</t>
+    <t>2017-05-24</t>
+  </si>
+  <si>
+    <t>2017-05-25</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Igor  Hnes</t>
+  </si>
+  <si>
+    <t>2017-05-07</t>
+  </si>
+  <si>
+    <t># 55 UTLS</t>
+  </si>
+  <si>
+    <t>2017-05-17</t>
+  </si>
+  <si>
+    <t>2017-05-26</t>
+  </si>
+  <si>
+    <t># 56 LRPM</t>
+  </si>
+  <si>
+    <t>2017-05-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI 4364 EM </t>
+  </si>
+  <si>
+    <t>Igor Gnes</t>
+  </si>
+  <si>
+    <t>2017-05-08</t>
+  </si>
+  <si>
+    <t># 57 EMR</t>
+  </si>
+  <si>
+    <t>2017-05-10</t>
   </si>
   <si>
     <t>2017-05-18</t>
   </si>
   <si>
-    <t># 17 BLS</t>
-  </si>
-  <si>
-    <t>Lviv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Igor Hnes Igor Hnes Igor Hnes </t>
+    <t xml:space="preserve">Igor  Gnes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ferrari </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Igor </t>
+  </si>
+  <si>
+    <t># 58 EMR</t>
+  </si>
+  <si>
+    <t>2017-05-11</t>
+  </si>
+  <si>
+    <t>2017-05-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АІ 4365 EM </t>
+  </si>
+  <si>
+    <t># 60 LRPM</t>
+  </si>
+  <si>
+    <t>Vika Savenets</t>
+  </si>
+  <si>
+    <t>2017-05-14</t>
+  </si>
+  <si>
+    <t># 61 BLS</t>
+  </si>
+  <si>
+    <t>2017-06-20</t>
+  </si>
+  <si>
+    <t>2017-06-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ferrari АІ 4365 EM AI 4364 EM </t>
+  </si>
+  <si>
+    <t># 62 LRPM</t>
+  </si>
+  <si>
+    <t>2017-05-22</t>
+  </si>
+  <si>
+    <t>2017-05-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АІ 4365 EM ferrari </t>
+  </si>
+  <si>
+    <t>2017-05-16</t>
   </si>
 </sst>
 </file>
@@ -120,9 +201,9 @@
     <col min="2" max="2" width="5.73828125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.5625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.5625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="28.96875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.29296875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.6484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="10.85546875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="29.1484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.0234375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.5625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -169,10 +250,10 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
@@ -183,25 +264,181 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>